<commit_message>
modificacion ejercicio 14 Excel
</commit_message>
<xml_diff>
--- a/INTRODUCCIÓN A LA INFORMÁTICA/Excel/Ejercicios_Resueltos/EJERCICIO 14_UNIDAD 1.xlsx
+++ b/INTRODUCCIÓN A LA INFORMÁTICA/Excel/Ejercicios_Resueltos/EJERCICIO 14_UNIDAD 1.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\UTN PACHECO\GUIA CURSO DE INGRESO 2024_bak\Resueltos_Guias_Repaso_TUP_2024_2025\INTRODUCCIÓN A LA INFORMÁTICA\Excel\Ejercicios_Resueltos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B475EE2-F596-438D-8B29-63F4B23E57A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FF44B6-EF42-4D43-B253-3A6E596CD066}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Datos-ejercicio14" sheetId="2" r:id="rId2"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId2"/>
+    <externalReference r:id="rId3"/>
   </externalReferences>
   <calcPr calcId="181029"/>
   <extLst>
@@ -213,7 +214,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -242,11 +243,27 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -314,9 +331,6 @@
           <cell r="B2" t="str">
             <v>Cristian Viamonte</v>
           </cell>
-          <cell r="F2">
-            <v>0.96</v>
-          </cell>
         </row>
         <row r="3">
           <cell r="A3" t="str">
@@ -324,9 +338,6 @@
           </cell>
           <cell r="B3" t="str">
             <v>Juliana Rosas</v>
-          </cell>
-          <cell r="G3">
-            <v>1.05</v>
           </cell>
         </row>
         <row r="4">
@@ -633,25 +644,24 @@
   <dimension ref="A1:N18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L19" sqref="L19"/>
+      <selection activeCell="F2" sqref="F2:F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="13.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="8" width="13.140625" style="10"/>
-    <col min="9" max="9" width="22.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="17.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="20.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="11.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="13.140625" style="10"/>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -673,30 +683,24 @@
       <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="M1" s="11" t="s">
-        <v>29</v>
-      </c>
-      <c r="N1" s="11" t="s">
-        <v>30</v>
-      </c>
+      <c r="L1" s="16"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="12" t="str">
+      <c r="B2" s="11" t="str">
         <f>IFERROR(VLOOKUP(A2,'[1]Datos-ejercicio14'!A2:B7,2,FALSE),"")</f>
         <v>Cristian Viamonte</v>
       </c>
@@ -709,33 +713,28 @@
       <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F2" s="13">
-        <f>IF(E2="DÉBITO",(IF(C2=$H$2,$J$2,$J$3)+(IF(D2="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E2="CRÉDITO",(IF(C2=$H$2,$J$2,$J$3)+(IF(D2="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
-        <v>33600</v>
-      </c>
-      <c r="H2" s="4" t="s">
+      <c r="F2" s="12">
+        <f>IF(E2="DÉBITO",(IF(C2=$J$2,$K$2,$K$3)+(IF(D2="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E2="CRÉDITO",(IF(C2=$J$2,$K$2,$K$3)+(IF(D2="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
+        <v>48000</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="I2" s="12" t="s">
+      <c r="J2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="J2" s="14">
+      <c r="K2" s="13">
         <v>25000</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="M2" s="12">
-        <f>(100-4)/100</f>
-        <v>0.96</v>
-      </c>
-      <c r="N2" s="12"/>
+      <c r="L2" s="18"/>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="str">
+      <c r="B3" s="11" t="str">
         <f>IFERROR(VLOOKUP(A3,'[1]Datos-ejercicio14'!A3:B8,2,FALSE),"")</f>
         <v>Juliana Rosas</v>
       </c>
@@ -748,33 +747,28 @@
       <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="13">
-        <f>IF(E3="DÉBITO",(IF(C3=$H$2,$J$2,$J$3)+(IF(D3="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E3="CRÉDITO",(IF(C3=$H$2,$J$2,$J$3)+(IF(D3="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F3" s="12">
+        <f>IF(E3="DÉBITO",(IF(C3=$J$2,$K$2,$K$3)+(IF(D3="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E3="CRÉDITO",(IF(C3=$J$2,$K$2,$K$3)+(IF(D3="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v>42000</v>
       </c>
-      <c r="H3" s="4" t="s">
+      <c r="I3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="I3" s="12" t="s">
+      <c r="J3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="J3" s="14">
+      <c r="K3" s="13">
         <v>40000</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="M3" s="12"/>
-      <c r="N3" s="12">
-        <f>(5/100)+1</f>
-        <v>1.05</v>
-      </c>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="19"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="12" t="str">
+      <c r="B4" s="11" t="str">
         <f>IFERROR(VLOOKUP(A4,'[1]Datos-ejercicio14'!A4:B9,2,FALSE),"")</f>
         <v>Estefano Moreno</v>
       </c>
@@ -787,25 +781,28 @@
       <c r="E4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="13">
-        <f>IF(E4="DÉBITO",(IF(C4=$H$2,$J$2,$J$3)+(IF(D4="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E4="CRÉDITO",(IF(C4=$H$2,$J$2,$J$3)+(IF(D4="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
-        <v>33600</v>
-      </c>
-      <c r="H4" s="5" t="s">
+      <c r="F4" s="12">
+        <f>IF(E4="DÉBITO",(IF(C4=$J$2,$K$2,$K$3)+(IF(D4="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E4="CRÉDITO",(IF(C4=$J$2,$K$2,$K$3)+(IF(D4="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
+        <v>48000</v>
+      </c>
+      <c r="I4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="I4" s="12" t="s">
+      <c r="J4" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="J4" s="6">
+      <c r="K4" s="6">
         <v>10000</v>
       </c>
+      <c r="L4" s="19"/>
+      <c r="M4" s="19"/>
+      <c r="N4" s="19"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="B5" s="12" t="str">
+      <c r="B5" s="11" t="str">
         <f>IFERROR(VLOOKUP(A5,'[1]Datos-ejercicio14'!A5:B10,2,FALSE),"")</f>
         <v>Agustina Perez</v>
       </c>
@@ -818,16 +815,19 @@
       <c r="E5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F5" s="13">
-        <f>IF(E5="DÉBITO",(IF(C5=$H$2,$J$2,$J$3)+(IF(D5="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E5="CRÉDITO",(IF(C5=$H$2,$J$2,$J$3)+(IF(D5="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
-        <v>26250</v>
-      </c>
+      <c r="F5" s="12">
+        <f>IF(E5="DÉBITO",(IF(C5=$J$2,$K$2,$K$3)+(IF(D5="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E5="CRÉDITO",(IF(C5=$J$2,$K$2,$K$3)+(IF(D5="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
+        <v>42000</v>
+      </c>
+      <c r="L5" s="19"/>
+      <c r="M5" s="19"/>
+      <c r="N5" s="19"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="B6" s="12" t="str">
+      <c r="B6" s="11" t="str">
         <f>IFERROR(VLOOKUP(A6,'[1]Datos-ejercicio14'!A6:B11,2,FALSE),"")</f>
         <v>Estella Castellano</v>
       </c>
@@ -840,16 +840,19 @@
       <c r="E6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F6" s="13">
-        <f>IF(E6="DÉBITO",(IF(C6=$H$2,$J$2,$J$3)+(IF(D6="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E6="CRÉDITO",(IF(C6=$H$2,$J$2,$J$3)+(IF(D6="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F6" s="12">
+        <f>IF(E6="DÉBITO",(IF(C6=$J$2,$K$2,$K$3)+(IF(D6="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E6="CRÉDITO",(IF(C6=$J$2,$K$2,$K$3)+(IF(D6="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v>52500</v>
       </c>
+      <c r="L6" s="19"/>
+      <c r="M6" s="19"/>
+      <c r="N6" s="19"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="12" t="str">
+      <c r="B7" s="11" t="str">
         <f>IFERROR(VLOOKUP(A7,'[1]Datos-ejercicio14'!A7:B12,2,FALSE),"")</f>
         <v>Franco Antón</v>
       </c>
@@ -862,128 +865,112 @@
       <c r="E7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="F7" s="13">
-        <f>IF(E7="DÉBITO",(IF(C7=$H$2,$J$2,$J$3)+(IF(D7="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E7="CRÉDITO",(IF(C7=$H$2,$J$2,$J$3)+(IF(D7="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F7" s="12">
+        <f>IF(E7="DÉBITO",(IF(C7=$J$2,$K$2,$K$3)+(IF(D7="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E7="CRÉDITO",(IF(C7=$J$2,$K$2,$K$3)+(IF(D7="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v>48000</v>
       </c>
-      <c r="H7" s="11" t="s">
+      <c r="I7" s="10" t="s">
         <v>25</v>
       </c>
-      <c r="I7" s="7">
+      <c r="J7" s="7">
         <f>AVERAGE(F2:F101)</f>
-        <v>39325</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="M7" s="1" t="s">
-        <v>1</v>
-      </c>
+        <v>46750</v>
+      </c>
+      <c r="L7" s="16"/>
+      <c r="M7" s="16"/>
+      <c r="N7" s="19"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="2"/>
-      <c r="B8" s="12" t="str">
+      <c r="B8" s="11" t="str">
         <f>IFERROR(VLOOKUP(A8,'[1]Datos-ejercicio14'!A8:B13,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="C8" s="12"/>
-      <c r="D8" s="12"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
       <c r="E8" s="3"/>
-      <c r="F8" s="13" t="str">
-        <f>IF(E8="DÉBITO",(IF(C8=$H$2,$J$2,$J$3)+(IF(D8="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E8="CRÉDITO",(IF(C8=$H$2,$J$2,$J$3)+(IF(D8="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F8" s="12" t="str">
+        <f>IF(E8="DÉBITO",(IF(C8=$J$2,$K$2,$K$3)+(IF(D8="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E8="CRÉDITO",(IF(C8=$J$2,$K$2,$K$3)+(IF(D8="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v/>
       </c>
-      <c r="H8" s="11" t="s">
+      <c r="I8" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="I8" s="2">
+      <c r="J8" s="2">
         <f>COUNTIF(D2:D101,"SÍ")</f>
         <v>4</v>
       </c>
-      <c r="L8" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="M8" s="12" t="s">
-        <v>31</v>
-      </c>
+      <c r="L8" s="20"/>
+      <c r="M8" s="19"/>
+      <c r="N8" s="19"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="2"/>
-      <c r="B9" s="12" t="str">
+      <c r="B9" s="11" t="str">
         <f>IFERROR(VLOOKUP(A9,'[1]Datos-ejercicio14'!A9:B14,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="C9" s="12"/>
-      <c r="D9" s="12"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
       <c r="E9" s="3"/>
-      <c r="F9" s="13" t="str">
-        <f>IF(E9="DÉBITO",(IF(C9=$H$2,$J$2,$J$3)+(IF(D9="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E9="CRÉDITO",(IF(C9=$H$2,$J$2,$J$3)+(IF(D9="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F9" s="12" t="str">
+        <f>IF(E9="DÉBITO",(IF(C9=$J$2,$K$2,$K$3)+(IF(D9="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E9="CRÉDITO",(IF(C9=$J$2,$K$2,$K$3)+(IF(D9="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v/>
       </c>
-      <c r="H9" s="11" t="s">
+      <c r="I9" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="I9" s="7">
+      <c r="J9" s="7">
         <f>MAX(F2:F101)</f>
         <v>52500</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="M9" s="12" t="s">
-        <v>33</v>
-      </c>
+      <c r="L9" s="20"/>
+      <c r="M9" s="19"/>
+      <c r="N9" s="19"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="2"/>
-      <c r="B10" s="12" t="str">
+      <c r="B10" s="11" t="str">
         <f>IFERROR(VLOOKUP(A10,'[1]Datos-ejercicio14'!A10:B15,2,FALSE),"")</f>
         <v/>
       </c>
-      <c r="C10" s="12"/>
-      <c r="D10" s="12"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
       <c r="E10" s="3"/>
-      <c r="F10" s="13" t="str">
-        <f>IF(E10="DÉBITO",(IF(C10=$H$2,$J$2,$J$3)+(IF(D10="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$F$2,IF(E10="CRÉDITO",(IF(C10=$H$2,$J$2,$J$3)+(IF(D10="SÍ",$J$4,0)))*'[1]Datos-ejercicio14'!$G$3,""))</f>
+      <c r="F10" s="12" t="str">
+        <f>IF(E10="DÉBITO",(IF(C10=$J$2,$K$2,$K$3)+(IF(D10="SÍ",$K$4,0)))*'Datos-ejercicio14'!$F$2,IF(E10="CRÉDITO",(IF(C10=$J$2,$K$2,$K$3)+(IF(D10="SÍ",$K$4,0)))*'Datos-ejercicio14'!$G$3,""))</f>
         <v/>
       </c>
-      <c r="H10" s="11" t="s">
+      <c r="I10" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="I10" s="2" t="str">
+      <c r="J10" s="2" t="str">
         <f>INDEX(B2:B101,MATCH(MAX(F2:F101),F2:F101,0))</f>
         <v>Estella Castellano</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>35</v>
-      </c>
+      <c r="L10" s="20"/>
+      <c r="M10" s="19"/>
+      <c r="N10" s="19"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L11" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>36</v>
-      </c>
+      <c r="L11" s="20"/>
+      <c r="M11" s="19"/>
+      <c r="N11" s="19"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L12" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>37</v>
-      </c>
+      <c r="L12" s="20"/>
+      <c r="M12" s="19"/>
+      <c r="N12" s="19"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="L13" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="M13" s="12" t="s">
-        <v>38</v>
-      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="19"/>
+      <c r="N13" s="19"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="L14" s="19"/>
+      <c r="M14" s="19"/>
+      <c r="N14" s="19"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="M15" s="8"/>
@@ -996,6 +983,113 @@
     </row>
     <row r="18" spans="13:13" x14ac:dyDescent="0.25">
       <c r="M18" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0F134222-0F1B-414C-8D0B-58D846E15186}">
+  <dimension ref="A1:G7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="11">
+        <f>(100-4)/100</f>
+        <v>0.96</v>
+      </c>
+      <c r="G2" s="11"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>33</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="11"/>
+      <c r="G3" s="11">
+        <f>(5/100)+1</f>
+        <v>1.05</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="E6" s="8"/>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E7" s="8"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>